<commit_message>
excel file data added, data fetching done in sheet 1(using VsCode)
</commit_message>
<xml_diff>
--- a/Implementation/Advanced_python_mini_project.xlsx
+++ b/Implementation/Advanced_python_mini_project.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t xml:space="preserve">PS_No.</t>
   </si>
@@ -81,6 +81,9 @@
   </si>
   <si>
     <t xml:space="preserve">Score19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Score20</t>
   </si>
 </sst>
 </file>
@@ -200,11 +203,11 @@
   </sheetPr>
   <dimension ref="A1:T17"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F27" activeCellId="0" sqref="F27"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="T12" activeCellId="0" sqref="T12:T16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.62890625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="14.28"/>
   </cols>
@@ -267,9 +270,11 @@
       <c r="S1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="2"/>
-    </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="T1" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="n">
         <v>99004351</v>
       </c>
@@ -326,6 +331,9 @@
       </c>
       <c r="S2" s="0" t="n">
         <v>23</v>
+      </c>
+      <c r="T2" s="0" t="n">
+        <v>91</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -386,6 +394,9 @@
       <c r="S3" s="0" t="n">
         <v>44</v>
       </c>
+      <c r="T3" s="0" t="n">
+        <v>43</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="n">
@@ -445,6 +456,9 @@
       <c r="S4" s="0" t="n">
         <v>91</v>
       </c>
+      <c r="T4" s="0" t="n">
+        <v>39</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="n">
@@ -504,6 +518,9 @@
       <c r="S5" s="0" t="n">
         <v>39</v>
       </c>
+      <c r="T5" s="0" t="n">
+        <v>39</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="n">
@@ -563,6 +580,9 @@
       <c r="S6" s="0" t="n">
         <v>91</v>
       </c>
+      <c r="T6" s="0" t="n">
+        <v>65</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="n">
@@ -622,6 +642,9 @@
       <c r="S7" s="0" t="n">
         <v>93</v>
       </c>
+      <c r="T7" s="0" t="n">
+        <v>75</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="n">
@@ -681,6 +704,9 @@
       <c r="S8" s="0" t="n">
         <v>43</v>
       </c>
+      <c r="T8" s="0" t="n">
+        <v>65</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="n">
@@ -740,6 +766,9 @@
       <c r="S9" s="0" t="n">
         <v>65</v>
       </c>
+      <c r="T9" s="0" t="n">
+        <v>39</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="n">
@@ -799,6 +828,9 @@
       <c r="S10" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="T10" s="0" t="n">
+        <v>43</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="n">
@@ -858,6 +890,9 @@
       <c r="S11" s="0" t="n">
         <v>91</v>
       </c>
+      <c r="T11" s="0" t="n">
+        <v>55</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="n">
@@ -917,6 +952,9 @@
       <c r="S12" s="0" t="n">
         <v>91</v>
       </c>
+      <c r="T12" s="0" t="n">
+        <v>93</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="n">
@@ -976,6 +1014,9 @@
       <c r="S13" s="0" t="n">
         <v>75</v>
       </c>
+      <c r="T13" s="0" t="n">
+        <v>99</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="n">
@@ -1035,6 +1076,9 @@
       <c r="S14" s="0" t="n">
         <v>65</v>
       </c>
+      <c r="T14" s="0" t="n">
+        <v>93</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="n">
@@ -1094,6 +1138,9 @@
       <c r="S15" s="0" t="n">
         <v>43</v>
       </c>
+      <c r="T15" s="0" t="n">
+        <v>39</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="n">
@@ -1152,6 +1199,9 @@
       </c>
       <c r="S16" s="0" t="n">
         <v>92</v>
+      </c>
+      <c r="T16" s="0" t="n">
+        <v>76</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1176,10 +1226,10 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="T12:T16 A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.62890625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -1199,10 +1249,10 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="T12:T16 A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.62890625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -1222,10 +1272,10 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="T12:T16 A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.62890625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -1245,10 +1295,10 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+      <selection pane="topLeft" activeCell="A4" activeCellId="1" sqref="T12:T16 A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.62890625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.43"/>
   </cols>

</xml_diff>